<commit_message>
update - guild merge
</commit_message>
<xml_diff>
--- a/data/BB8.xlsx
+++ b/data/BB8.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wojciech.kawecki/GitHub/swgoh-bots/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F8B228-6893-4842-B6C6-C87E0CC6B348}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC3B37E-2960-C947-A932-12171D8E02D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
   </sheets>
   <calcPr calcId="171026" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Selected Rows &amp; Columns" guid="{C889AC74-BC82-49E8-BA01-AB64462BFCF2}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="Selected Rows &amp; Columns" guid="{C889AC74-BC82-49E8-BA01-AB64462BFCF2}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -282,15 +282,29 @@
   </si>
   <si>
     <t>mahargobroh</t>
+  </si>
+  <si>
+    <t>Yodazmey</t>
+  </si>
+  <si>
+    <t>yodazmey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -407,26 +421,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -551,12 +566,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D38" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A1:D38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:D38">
-    <sortCondition ref="D2:D38"/>
-    <sortCondition ref="B2:B38"/>
-    <sortCondition ref="A2:A38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D39" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:D39" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:D39">
+    <sortCondition ref="D2:D39"/>
+    <sortCondition ref="B2:B39"/>
+    <sortCondition ref="A2:A39"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="3"/>
@@ -569,9 +584,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -609,7 +624,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -715,7 +730,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -865,20 +880,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.87109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.9921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.859375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.89453125" style="4"/>
+    <col min="1" max="1" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1070,54 +1085,54 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B16" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3">
+      <c r="D16" s="12">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D18" s="3">
         <v>16</v>
@@ -1125,13 +1140,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="D19" s="3">
         <v>16</v>
@@ -1139,13 +1154,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="D20" s="3">
         <v>16</v>
@@ -1153,13 +1168,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D21" s="3">
         <v>16</v>
@@ -1167,60 +1182,62 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>66</v>
+        <v>14</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="D22" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B24" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C24" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D24" s="10">
         <v>16</v>
       </c>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>41</v>
@@ -1231,96 +1248,94 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D29" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B30" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C30" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="14">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="13">
+      <c r="D30" s="14">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="3">
-        <v>21</v>
+        <v>74</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="13">
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D33" s="3">
         <v>22</v>
@@ -1328,13 +1343,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D34" s="3">
         <v>22</v>
@@ -1342,13 +1357,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D35" s="3">
         <v>22</v>
@@ -1356,13 +1371,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D36" s="3">
         <v>22</v>
@@ -1370,35 +1385,43 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D37" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D39" s="9">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
@@ -1435,6 +1458,12 @@
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>